<commit_message>
upload naver shopping crawl
</commit_message>
<xml_diff>
--- a/수집_대상_카테고리.xlsx
+++ b/수집_대상_카테고리.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\seho\220cordncode\Naver_Shopping_Crawl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\seho\Naver_Shopping_Crawl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DB463C-6537-4479-86E2-BC040A9B1DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B63A8C8-8DD6-4585-8FAC-7811E645CAB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="22470" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="419">
   <si>
     <t>category_id</t>
   </si>
@@ -1238,10 +1230,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>자동만</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>디지털/가전</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1278,10 +1266,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>전동,배터리,자동</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>휴대폰액세서리</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1347,6 +1331,58 @@
   </si>
   <si>
     <t>보틀워머</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>생활</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>건강</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주방용품</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>커피용품</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>우유거품기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>위생/건강용품</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>콧물흡입기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1354,7 +1390,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1375,6 +1411,26 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1412,7 +1468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1420,6 +1476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1722,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F192"/>
+  <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="K192" sqref="K192"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4216,7 +4273,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>50001119</v>
       </c>
@@ -4230,7 +4287,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>50000063</v>
       </c>
@@ -4241,7 +4298,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>50001603</v>
       </c>
@@ -4255,7 +4312,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>50001821</v>
       </c>
@@ -4269,7 +4326,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>50008649</v>
       </c>
@@ -4285,28 +4342,25 @@
       <c r="E181" t="s">
         <v>386</v>
       </c>
-      <c r="F181" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>50001226</v>
       </c>
       <c r="B182" t="s">
+        <v>387</v>
+      </c>
+      <c r="C182" t="s">
         <v>388</v>
       </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>389</v>
       </c>
-      <c r="D182" t="s">
+      <c r="E182" t="s">
         <v>390</v>
       </c>
-      <c r="E182" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>50006669</v>
       </c>
@@ -4317,13 +4371,13 @@
         <v>340</v>
       </c>
       <c r="D183" t="s">
+        <v>391</v>
+      </c>
+      <c r="E183" t="s">
         <v>392</v>
       </c>
-      <c r="E183" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>50004575</v>
       </c>
@@ -4334,16 +4388,13 @@
         <v>364</v>
       </c>
       <c r="D184" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E184" t="s">
-        <v>404</v>
-      </c>
-      <c r="F184" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>50002477</v>
       </c>
@@ -4351,36 +4402,33 @@
         <v>350</v>
       </c>
       <c r="C185" t="s">
+        <v>393</v>
+      </c>
+      <c r="D185" t="s">
         <v>394</v>
       </c>
-      <c r="D185" t="s">
+      <c r="E185" t="s">
         <v>395</v>
       </c>
-      <c r="E185" t="s">
-        <v>396</v>
-      </c>
-      <c r="F185" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>50004603</v>
       </c>
       <c r="B186" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C186" t="s">
+        <v>396</v>
+      </c>
+      <c r="D186" t="s">
+        <v>397</v>
+      </c>
+      <c r="E186" t="s">
         <v>398</v>
       </c>
-      <c r="D186" t="s">
-        <v>399</v>
-      </c>
-      <c r="E186" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>50002707</v>
       </c>
@@ -4388,16 +4436,16 @@
         <v>350</v>
       </c>
       <c r="C187" t="s">
+        <v>399</v>
+      </c>
+      <c r="D187" t="s">
+        <v>400</v>
+      </c>
+      <c r="E187" t="s">
         <v>401</v>
       </c>
-      <c r="D187" t="s">
-        <v>402</v>
-      </c>
-      <c r="E187" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>50003330</v>
       </c>
@@ -4408,14 +4456,14 @@
         <v>375</v>
       </c>
       <c r="D188" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E188" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" s="2">
         <v>50003331</v>
       </c>
       <c r="B189" t="s">
@@ -4425,30 +4473,30 @@
         <v>375</v>
       </c>
       <c r="D189" t="s">
+        <v>404</v>
+      </c>
+      <c r="E189" t="s">
         <v>406</v>
       </c>
-      <c r="E189" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>50002347</v>
       </c>
       <c r="B190" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C190" t="s">
         <v>354</v>
       </c>
       <c r="D190" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E190" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>50000367</v>
       </c>
@@ -4456,13 +4504,13 @@
         <v>346</v>
       </c>
       <c r="C191" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D191" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>50000675</v>
       </c>
@@ -4470,10 +4518,41 @@
         <v>346</v>
       </c>
       <c r="C192" t="s">
+        <v>411</v>
+      </c>
+      <c r="D192" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="2">
+        <v>50004796</v>
+      </c>
+      <c r="B193" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="D192" t="s">
+      <c r="C193" t="s">
         <v>414</v>
+      </c>
+      <c r="D193" t="s">
+        <v>415</v>
+      </c>
+      <c r="E193" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="2">
+        <v>50000614</v>
+      </c>
+      <c r="B194" t="s">
+        <v>346</v>
+      </c>
+      <c r="C194" t="s">
+        <v>417</v>
+      </c>
+      <c r="D194" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>